<commit_message>
Initial display implementation of placement versus marketvalue data
</commit_message>
<xml_diff>
--- a/data/BundesligaDaten.xlsx
+++ b/data/BundesligaDaten.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\WebstormProjects\FootballClubEfficiency\csvFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\WebstormProjects\FootballClubEfficiency\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="135">
   <si>
     <t>Verein</t>
   </si>
@@ -256,6 +256,180 @@
   </si>
   <si>
     <t>Jahr</t>
+  </si>
+  <si>
+    <t>Legionäre</t>
+  </si>
+  <si>
+    <t>23,5 Jahre</t>
+  </si>
+  <si>
+    <t>2,58 Mrd. €</t>
+  </si>
+  <si>
+    <t>4,01 Mio. €</t>
+  </si>
+  <si>
+    <t>595,40 Mio. €</t>
+  </si>
+  <si>
+    <t>18,04 Mio. €</t>
+  </si>
+  <si>
+    <t>Borussia Dortmund</t>
+  </si>
+  <si>
+    <t>24,2</t>
+  </si>
+  <si>
+    <t>321,05 Mio. €</t>
+  </si>
+  <si>
+    <t>10,36 Mio. €</t>
+  </si>
+  <si>
+    <t>22,8</t>
+  </si>
+  <si>
+    <t>244,58 Mio. €</t>
+  </si>
+  <si>
+    <t>6,27 Mio. €</t>
+  </si>
+  <si>
+    <t>23,7</t>
+  </si>
+  <si>
+    <t>238,75 Mio. €</t>
+  </si>
+  <si>
+    <t>6,12 Mio. €</t>
+  </si>
+  <si>
+    <t>23,5</t>
+  </si>
+  <si>
+    <t>225,35 Mio. €</t>
+  </si>
+  <si>
+    <t>5,24 Mio. €</t>
+  </si>
+  <si>
+    <t>23,4</t>
+  </si>
+  <si>
+    <t>155,80 Mio. €</t>
+  </si>
+  <si>
+    <t>4,72 Mio. €</t>
+  </si>
+  <si>
+    <t>23,6</t>
+  </si>
+  <si>
+    <t>94,98 Mio. €</t>
+  </si>
+  <si>
+    <t>2,50 Mio. €</t>
+  </si>
+  <si>
+    <t>23,3</t>
+  </si>
+  <si>
+    <t>85,70 Mio. €</t>
+  </si>
+  <si>
+    <t>2,20 Mio. €</t>
+  </si>
+  <si>
+    <t>77,40 Mio. €</t>
+  </si>
+  <si>
+    <t>2,58 Mio. €</t>
+  </si>
+  <si>
+    <t>76,55 Mio. €</t>
+  </si>
+  <si>
+    <t>2,32 Mio. €</t>
+  </si>
+  <si>
+    <t>24,0</t>
+  </si>
+  <si>
+    <t>75,98 Mio. €</t>
+  </si>
+  <si>
+    <t>2,30 Mio. €</t>
+  </si>
+  <si>
+    <t>24,5</t>
+  </si>
+  <si>
+    <t>75,08 Mio. €</t>
+  </si>
+  <si>
+    <t>1,83 Mio. €</t>
+  </si>
+  <si>
+    <t>RasenBallsport Leipzig  </t>
+  </si>
+  <si>
+    <t>22,6</t>
+  </si>
+  <si>
+    <t>69,18 Mio. €</t>
+  </si>
+  <si>
+    <t>2,10 Mio. €</t>
+  </si>
+  <si>
+    <t>69,00 Mio. €</t>
+  </si>
+  <si>
+    <t>1,86 Mio. €</t>
+  </si>
+  <si>
+    <t>23,1</t>
+  </si>
+  <si>
+    <t>66,10 Mio. €</t>
+  </si>
+  <si>
+    <t>1,89 Mio. €</t>
+  </si>
+  <si>
+    <t>40,25 Mio. €</t>
+  </si>
+  <si>
+    <t>1,12 Mio. €</t>
+  </si>
+  <si>
+    <t>FC Ingolstadt 04</t>
+  </si>
+  <si>
+    <t>23,8</t>
+  </si>
+  <si>
+    <t>36,68 Mio. €</t>
+  </si>
+  <si>
+    <t>1,15 Mio. €</t>
+  </si>
+  <si>
+    <t>SV Darmstadt 98</t>
+  </si>
+  <si>
+    <t>32,83 Mio. €</t>
+  </si>
+  <si>
+    <t>842 Tsd. €</t>
+  </si>
+  <si>
+    <t>FC Bayern München</t>
+  </si>
+  <si>
+    <t>SC Freiburg  Deutscher Zweitligameister 15/16</t>
   </si>
 </sst>
 </file>
@@ -1657,10 +1831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="O3" sqref="O3:O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,9 +1846,15 @@
     <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="66.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>72</v>
       </c>
@@ -1696,8 +1876,23 @@
       <c r="G1" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>73</v>
@@ -1717,8 +1912,23 @@
       <c r="G2" s="1">
         <v>2017</v>
       </c>
+      <c r="K2">
+        <v>644</v>
+      </c>
+      <c r="L2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2">
+        <v>320</v>
+      </c>
+      <c r="N2" t="s">
+        <v>79</v>
+      </c>
+      <c r="O2" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
         <v>74</v>
@@ -1738,8 +1948,29 @@
       <c r="G3" s="1">
         <v>2017</v>
       </c>
+      <c r="I3" t="s">
+        <v>133</v>
+      </c>
+      <c r="J3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K3">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>81</v>
+      </c>
+      <c r="O3" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="2" t="s">
         <v>11</v>
@@ -1759,8 +1990,29 @@
       <c r="G4" s="1">
         <v>2017</v>
       </c>
+      <c r="I4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4">
+        <v>31</v>
+      </c>
+      <c r="L4" t="s">
+        <v>84</v>
+      </c>
+      <c r="M4">
+        <v>17</v>
+      </c>
+      <c r="N4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O4" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="2" t="s">
         <v>15</v>
@@ -1780,8 +2032,29 @@
       <c r="G5" s="1">
         <v>2017</v>
       </c>
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s">
+        <v>87</v>
+      </c>
+      <c r="M5">
+        <v>21</v>
+      </c>
+      <c r="N5" t="s">
+        <v>88</v>
+      </c>
+      <c r="O5" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="2" t="s">
         <v>19</v>
@@ -1801,8 +2074,29 @@
       <c r="G6" s="1">
         <v>2017</v>
       </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6">
+        <v>39</v>
+      </c>
+      <c r="L6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M6">
+        <v>22</v>
+      </c>
+      <c r="N6" t="s">
+        <v>91</v>
+      </c>
+      <c r="O6" t="s">
+        <v>92</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -1822,8 +2116,29 @@
       <c r="G7" s="1">
         <v>2017</v>
       </c>
+      <c r="I7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7">
+        <v>43</v>
+      </c>
+      <c r="L7" t="s">
+        <v>93</v>
+      </c>
+      <c r="M7">
+        <v>21</v>
+      </c>
+      <c r="N7" t="s">
+        <v>94</v>
+      </c>
+      <c r="O7" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="2" t="s">
         <v>27</v>
@@ -1843,8 +2158,29 @@
       <c r="G8" s="1">
         <v>2017</v>
       </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8">
+        <v>33</v>
+      </c>
+      <c r="L8" t="s">
+        <v>96</v>
+      </c>
+      <c r="M8">
+        <v>15</v>
+      </c>
+      <c r="N8" t="s">
+        <v>97</v>
+      </c>
+      <c r="O8" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="2" t="s">
         <v>31</v>
@@ -1864,8 +2200,29 @@
       <c r="G9" s="1">
         <v>2017</v>
       </c>
+      <c r="I9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9">
+        <v>38</v>
+      </c>
+      <c r="L9" t="s">
+        <v>99</v>
+      </c>
+      <c r="M9">
+        <v>20</v>
+      </c>
+      <c r="N9" t="s">
+        <v>100</v>
+      </c>
+      <c r="O9" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="2" t="s">
         <v>35</v>
@@ -1885,8 +2242,29 @@
       <c r="G10" s="1">
         <v>2017</v>
       </c>
+      <c r="I10" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10">
+        <v>39</v>
+      </c>
+      <c r="L10" t="s">
+        <v>102</v>
+      </c>
+      <c r="M10">
+        <v>22</v>
+      </c>
+      <c r="N10" t="s">
+        <v>103</v>
+      </c>
+      <c r="O10" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="2" t="s">
         <v>39</v>
@@ -1906,8 +2284,29 @@
       <c r="G11" s="1">
         <v>2017</v>
       </c>
+      <c r="I11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11">
+        <v>30</v>
+      </c>
+      <c r="L11" t="s">
+        <v>12</v>
+      </c>
+      <c r="M11">
+        <v>14</v>
+      </c>
+      <c r="N11" t="s">
+        <v>105</v>
+      </c>
+      <c r="O11" t="s">
+        <v>106</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="2" t="s">
         <v>43</v>
@@ -1927,8 +2326,29 @@
       <c r="G12" s="1">
         <v>2017</v>
       </c>
+      <c r="I12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12">
+        <v>33</v>
+      </c>
+      <c r="L12" t="s">
+        <v>93</v>
+      </c>
+      <c r="M12">
+        <v>15</v>
+      </c>
+      <c r="N12" t="s">
+        <v>107</v>
+      </c>
+      <c r="O12" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
         <v>75</v>
@@ -1948,8 +2368,29 @@
       <c r="G13" s="1">
         <v>2017</v>
       </c>
+      <c r="I13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13">
+        <v>33</v>
+      </c>
+      <c r="L13" t="s">
+        <v>109</v>
+      </c>
+      <c r="M13">
+        <v>14</v>
+      </c>
+      <c r="N13" t="s">
+        <v>110</v>
+      </c>
+      <c r="O13" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="2" t="s">
         <v>49</v>
@@ -1969,8 +2410,29 @@
       <c r="G14" s="1">
         <v>2017</v>
       </c>
+      <c r="I14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" t="s">
+        <v>49</v>
+      </c>
+      <c r="K14">
+        <v>41</v>
+      </c>
+      <c r="L14" t="s">
+        <v>112</v>
+      </c>
+      <c r="M14">
+        <v>20</v>
+      </c>
+      <c r="N14" t="s">
+        <v>113</v>
+      </c>
+      <c r="O14" t="s">
+        <v>114</v>
+      </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="2" t="s">
         <v>53</v>
@@ -1990,8 +2452,29 @@
       <c r="G15" s="1">
         <v>2017</v>
       </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" t="s">
+        <v>115</v>
+      </c>
+      <c r="K15">
+        <v>33</v>
+      </c>
+      <c r="L15" t="s">
+        <v>116</v>
+      </c>
+      <c r="M15">
+        <v>15</v>
+      </c>
+      <c r="N15" t="s">
+        <v>117</v>
+      </c>
+      <c r="O15" t="s">
+        <v>118</v>
+      </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="2" t="s">
         <v>57</v>
@@ -2011,8 +2494,29 @@
       <c r="G16" s="1">
         <v>2017</v>
       </c>
+      <c r="I16" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16">
+        <v>37</v>
+      </c>
+      <c r="L16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M16">
+        <v>21</v>
+      </c>
+      <c r="N16" t="s">
+        <v>119</v>
+      </c>
+      <c r="O16" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="2" t="s">
         <v>61</v>
@@ -2032,8 +2536,29 @@
       <c r="G17" s="1">
         <v>2017</v>
       </c>
+      <c r="I17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17">
+        <v>35</v>
+      </c>
+      <c r="L17" t="s">
+        <v>121</v>
+      </c>
+      <c r="M17">
+        <v>21</v>
+      </c>
+      <c r="N17" t="s">
+        <v>122</v>
+      </c>
+      <c r="O17" t="s">
+        <v>123</v>
+      </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="2" t="s">
         <v>65</v>
@@ -2053,8 +2578,29 @@
       <c r="G18" s="1">
         <v>2017</v>
       </c>
+      <c r="I18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" t="s">
+        <v>134</v>
+      </c>
+      <c r="K18">
+        <v>36</v>
+      </c>
+      <c r="L18" t="s">
+        <v>109</v>
+      </c>
+      <c r="M18">
+        <v>13</v>
+      </c>
+      <c r="N18" t="s">
+        <v>124</v>
+      </c>
+      <c r="O18" t="s">
+        <v>125</v>
+      </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="2" t="s">
         <v>68</v>
@@ -2074,10 +2620,55 @@
       <c r="G19" s="1">
         <v>2017</v>
       </c>
+      <c r="I19" t="s">
+        <v>126</v>
+      </c>
+      <c r="J19" t="s">
+        <v>126</v>
+      </c>
+      <c r="K19">
+        <v>32</v>
+      </c>
+      <c r="L19" t="s">
+        <v>127</v>
+      </c>
+      <c r="M19">
+        <v>15</v>
+      </c>
+      <c r="N19" t="s">
+        <v>128</v>
+      </c>
+      <c r="O19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>130</v>
+      </c>
+      <c r="J20" t="s">
+        <v>130</v>
+      </c>
+      <c r="K20">
+        <v>39</v>
+      </c>
+      <c r="L20" t="s">
+        <v>8</v>
+      </c>
+      <c r="M20">
+        <v>17</v>
+      </c>
+      <c r="N20" t="s">
+        <v>131</v>
+      </c>
+      <c r="O20" t="s">
+        <v>132</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>